<commit_message>
docs: terminate fourth sprint
</commit_message>
<xml_diff>
--- a/docs/process/fourth-sprint-backlog.xlsx
+++ b/docs/process/fourth-sprint-backlog.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
   <si>
     <t xml:space="preserve">Remaining effort at the end of the day ... </t>
   </si>
@@ -37,6 +37,9 @@
     <t>Felice</t>
   </si>
   <si>
+    <t>/</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <rFont val="Arial"/>
@@ -54,10 +57,13 @@
     </r>
   </si>
   <si>
-    <t>Cesario, Kentpayeva</t>
+    <t>Cesario</t>
   </si>
   <si>
     <t>Annullamento delle sottoscrizioni agli eventi</t>
+  </si>
+  <si>
+    <t>Kentpayeva</t>
   </si>
   <si>
     <t>Rimozione della possibilità di chiudere la finestra della promozione</t>
@@ -73,6 +79,9 @@
   </si>
   <si>
     <t>Ottimizzazione dell'analisi della prima mossa</t>
+  </si>
+  <si>
+    <t>Cesario, Kentpayeva</t>
   </si>
   <si>
     <t>Test refactoring</t>
@@ -607,12 +616,24 @@
       <c r="E4" s="12">
         <v>1.0</v>
       </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
+      <c r="F4" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="G4" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="H4" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="I4" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="J4" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="L4" s="13"/>
       <c r="M4" s="14"/>
       <c r="N4" s="14"/>
@@ -626,21 +647,35 @@
       <c r="A5" s="9"/>
       <c r="B5" s="15"/>
       <c r="C5" s="11" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E5" s="12">
         <v>3.0</v>
       </c>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
+      <c r="F5" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="G5" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="H5" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="I5" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="J5" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="K5" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="M5" s="14"/>
       <c r="N5" s="14"/>
       <c r="O5" s="14"/>
@@ -653,21 +688,35 @@
       <c r="A6" s="9"/>
       <c r="B6" s="15"/>
       <c r="C6" s="11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E6" s="12">
         <v>1.0</v>
       </c>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
+      <c r="F6" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="G6" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="H6" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="I6" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="J6" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="K6" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="L6" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="M6" s="14"/>
       <c r="N6" s="14"/>
       <c r="O6" s="14"/>
@@ -680,7 +729,7 @@
       <c r="A7" s="9"/>
       <c r="B7" s="15"/>
       <c r="C7" s="11" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>7</v>
@@ -688,7 +737,9 @@
       <c r="E7" s="12">
         <v>1.0</v>
       </c>
-      <c r="F7" s="12"/>
+      <c r="F7" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="G7" s="12"/>
       <c r="H7" s="13"/>
       <c r="I7" s="13"/>
@@ -707,16 +758,20 @@
       <c r="A8" s="9"/>
       <c r="B8" s="15"/>
       <c r="C8" s="11" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E8" s="12">
         <v>1.0</v>
       </c>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
+      <c r="F8" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="H8" s="13"/>
       <c r="I8" s="13"/>
       <c r="J8" s="13"/>
@@ -734,15 +789,17 @@
       <c r="A9" s="9"/>
       <c r="B9" s="15"/>
       <c r="C9" s="11" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E9" s="12">
         <v>1.0</v>
       </c>
-      <c r="F9" s="12"/>
+      <c r="F9" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="G9" s="12"/>
       <c r="H9" s="13"/>
       <c r="I9" s="13"/>
@@ -761,21 +818,35 @@
       <c r="A10" s="9"/>
       <c r="B10" s="15"/>
       <c r="C10" s="16" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E10" s="12">
         <v>2.0</v>
       </c>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
+      <c r="F10" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="G10" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="H10" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="I10" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="J10" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="K10" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="L10" s="12">
+        <v>2.0</v>
+      </c>
       <c r="M10" s="14"/>
       <c r="N10" s="14"/>
       <c r="O10" s="14"/>
@@ -788,21 +859,35 @@
       <c r="A11" s="9"/>
       <c r="B11" s="15"/>
       <c r="C11" s="11" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E11" s="12">
         <v>3.0</v>
       </c>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
+      <c r="F11" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="G11" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="H11" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="I11" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="J11" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="K11" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="L11" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="M11" s="14"/>
       <c r="N11" s="14"/>
       <c r="O11" s="14"/>
@@ -815,18 +900,26 @@
       <c r="A12" s="9"/>
       <c r="B12" s="15"/>
       <c r="C12" s="11" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E12" s="12">
         <v>3.0</v>
       </c>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
+      <c r="F12" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="G12" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="H12" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="J12" s="13"/>
       <c r="K12" s="13"/>
       <c r="L12" s="13"/>
@@ -842,21 +935,35 @@
       <c r="A13" s="9"/>
       <c r="B13" s="17"/>
       <c r="C13" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="12" t="s">
         <v>20</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>17</v>
       </c>
       <c r="E13" s="12">
         <v>3.0</v>
       </c>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
+      <c r="F13" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="G13" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="H13" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="I13" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="J13" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="K13" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="L13" s="12">
+        <v>2.0</v>
+      </c>
       <c r="M13" s="14"/>
       <c r="N13" s="14"/>
       <c r="O13" s="14"/>
@@ -868,10 +975,10 @@
     <row r="14">
       <c r="A14" s="9"/>
       <c r="B14" s="18" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>7</v>
@@ -879,9 +986,13 @@
       <c r="E14" s="12">
         <v>2.0</v>
       </c>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="13"/>
+      <c r="F14" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14" s="12"/>
       <c r="I14" s="13"/>
       <c r="J14" s="13"/>
       <c r="K14" s="13"/>

</xml_diff>